<commit_message>
Backend - Busq vuelos
</commit_message>
<xml_diff>
--- a/carga manual de vuelos.xlsx
+++ b/carga manual de vuelos.xlsx
@@ -148,14 +148,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,7 +438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -457,17 +457,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
       <c r="J1" t="s">
         <v>8</v>
       </c>
@@ -503,7 +503,7 @@
       <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="N2" t="s">
@@ -520,10 +520,10 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
@@ -547,35 +547,35 @@
       <c r="I3">
         <v>1</v>
       </c>
-      <c r="J3" s="3" t="str">
+      <c r="J3" s="2" t="str">
         <f>CONCATENATE("(",A3,",",B3,",",C3,",",D3,",",E3,",",F3,",",G3,",",H3,",",I3,")")</f>
         <v>('brrio01','LAN','buenos aires','bue-eze','rio de janeiro','bra-gig','06-23-2019',NULL,1)</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="N3">
         <v>3</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="Q3">
         <v>450</v>
       </c>
-      <c r="R3" s="3" t="str">
+      <c r="R3" s="2" t="str">
         <f>CONCATENATE("(",M3,",",N3,",",O3,",",P3,",",Q3,")")</f>
         <v>('brrio01',3,'09:00:00','12:00:00',450)</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="195" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
@@ -599,26 +599,26 @@
       <c r="I4">
         <v>1</v>
       </c>
-      <c r="J4" s="3" t="str">
+      <c r="J4" s="2" t="str">
         <f>CONCATENATE("(",A4,",",B4,",",C4,",",D4,",",E4,",",F4,",",G4,",",H4,",",I4,")")</f>
         <v>('brrio02','LAN','rio de janeiro','bra-gig','buenos aires','bue-eze','06-23-2019',NULL,1)</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="N4">
         <v>3</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="P4" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Q4">
         <v>490</v>
       </c>
-      <c r="R4" s="3" t="str">
+      <c r="R4" s="2" t="str">
         <f>CONCATENATE("(",M4,",",N4,",",O4,",",P4,",",Q4,")")</f>
         <v>('brrio02',3,'15:00:00','18:00:00',490)</v>
       </c>

</xml_diff>

<commit_message>
Actualizacion de base de datos
</commit_message>
<xml_diff>
--- a/carga manual de vuelos.xlsx
+++ b/carga manual de vuelos.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facultad\ort\TP Final c21A\PNT2_Sistema_Reservas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Usuario\Desktop\ORT2019\ProyectoORT\PNT2_Sistema_Reservas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6555"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="6552"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,20 +24,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="65">
   <si>
     <t>'LAN'</t>
   </si>
   <si>
-    <t>'buenos aires'</t>
-  </si>
-  <si>
     <t>'bue-eze'</t>
   </si>
   <si>
-    <t>'rio de janeiro'</t>
-  </si>
-  <si>
     <t>'bra-gig'</t>
   </si>
   <si>
@@ -111,12 +105,126 @@
   </si>
   <si>
     <t>'12:00:00'</t>
+  </si>
+  <si>
+    <t>'DL101'</t>
+  </si>
+  <si>
+    <t>'Delta'</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro'</t>
+  </si>
+  <si>
+    <t>Buenos Aires'</t>
+  </si>
+  <si>
+    <t>'Buenos Aires'</t>
+  </si>
+  <si>
+    <t>'Atlanta'</t>
+  </si>
+  <si>
+    <t>bue-eze'</t>
+  </si>
+  <si>
+    <t>'atl-atl'</t>
+  </si>
+  <si>
+    <t>'08-26-2019'</t>
+  </si>
+  <si>
+    <t>'20:35:00'</t>
+  </si>
+  <si>
+    <t>'06:35:00'</t>
+  </si>
+  <si>
+    <t>'DL102'</t>
+  </si>
+  <si>
+    <t>'08-30-2019'</t>
+  </si>
+  <si>
+    <t>'AR2880'</t>
+  </si>
+  <si>
+    <t>'Aerolineas Argentinas'</t>
+  </si>
+  <si>
+    <t>'bue-aep'</t>
+  </si>
+  <si>
+    <t>'ssj-juy'</t>
+  </si>
+  <si>
+    <t>'05-29-2019'</t>
+  </si>
+  <si>
+    <t>'16:45:00'</t>
+  </si>
+  <si>
+    <t>'18:45:00'</t>
+  </si>
+  <si>
+    <t>'AR2881'</t>
+  </si>
+  <si>
+    <t>'San Salvador de Jujuy'</t>
+  </si>
+  <si>
+    <t>'05-30-2019'</t>
+  </si>
+  <si>
+    <t>'AR2550'</t>
+  </si>
+  <si>
+    <t>'AR2551'</t>
+  </si>
+  <si>
+    <t>'AR2600'</t>
+  </si>
+  <si>
+    <t>'AR2601'</t>
+  </si>
+  <si>
+    <t>'Ushuaia'</t>
+  </si>
+  <si>
+    <t>'tdf-uha'</t>
+  </si>
+  <si>
+    <t>'06-30-2019'</t>
+  </si>
+  <si>
+    <t>'07-30-2019'</t>
+  </si>
+  <si>
+    <t>'20:45:00'</t>
+  </si>
+  <si>
+    <t>'19:45:00'</t>
+  </si>
+  <si>
+    <t>'21:45:00'</t>
+  </si>
+  <si>
+    <t>'Mendoza'</t>
+  </si>
+  <si>
+    <t>'mdz-mdz'</t>
+  </si>
+  <si>
+    <t>'17:45:00'</t>
+  </si>
+  <si>
+    <t>'23:45:00'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -174,7 +282,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -436,29 +544,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -469,99 +577,99 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="N2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
+    <row r="3" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="I2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>4</v>
-      </c>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" t="s">
-        <v>6</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3" s="2" t="str">
         <f>CONCATENATE("(",A3,",",B3,",",C3,",",D3,",",E3,",",F3,",",G3,",",H3,",",I3,")")</f>
-        <v>('brrio01','LAN','buenos aires','bue-eze','rio de janeiro','bra-gig','06-23-2019',NULL,1)</v>
+        <v>('brrio01','LAN',Buenos Aires','bue-eze',Rio de Janeiro','bra-gig','06-23-2019',NULL,1)</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N3">
         <v>3</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Q3">
         <v>450</v>
@@ -571,49 +679,49 @@
         <v>('brrio01',3,'09:00:00','12:00:00',450)</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H4" t="s">
         <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" t="s">
-        <v>6</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" s="2" t="str">
         <f>CONCATENATE("(",A4,",",B4,",",C4,",",D4,",",E4,",",F4,",",G4,",",H4,",",I4,")")</f>
-        <v>('brrio02','LAN','rio de janeiro','bra-gig','buenos aires','bue-eze','06-23-2019',NULL,1)</v>
+        <v>('brrio02','LAN',Rio de Janeiro','bra-gig',Buenos Aires',bue-eze','06-23-2019',NULL,1)</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N4">
         <v>3</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q4">
         <v>490</v>
@@ -621,6 +729,422 @@
       <c r="R4" s="2" t="str">
         <f>CONCATENATE("(",M4,",",N4,",",O4,",",P4,",",Q4,")")</f>
         <v>('brrio02',3,'15:00:00','18:00:00',490)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="str">
+        <f>CONCATENATE("(",A5,",",B5,",",C5,",",D5,",",E5,",",F5,",",G5,",",H5,",",I5,")")</f>
+        <v>('DL101','Delta','Buenos Aires','bue-eze','Atlanta','atl-atl','08-26-2019',NULL,1)</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5">
+        <v>10</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q5">
+        <v>1250</v>
+      </c>
+      <c r="R5" s="2" t="str">
+        <f>CONCATENATE("(",M5,",",N5,",",O5,",",P5,",",Q5,")")</f>
+        <v>('DL101',10,'20:35:00','06:35:00',1250)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2" t="str">
+        <f>CONCATENATE("(",A6,",",B6,",",C6,",",D6,",",E6,",",F6,",",G6,",",H6,",",I6,")")</f>
+        <v>('DL102','Delta','Atlanta','atl-atl','Buenos Aires','bue-eze','08-30-2019',NULL,1)</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N6">
+        <v>10</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q6">
+        <v>1300</v>
+      </c>
+      <c r="R6" s="2" t="str">
+        <f t="shared" ref="R6:R8" si="0">CONCATENATE("(",M6,",",N6,",",O6,",",P6,",",Q6,")")</f>
+        <v>('DL102',10,'20:35:00','06:35:00',1300)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2" t="str">
+        <f>CONCATENATE("(",A7,",",B7,",",C7,",",D7,",",E7,",",F7,",",G7,",",H7,",",I7,")")</f>
+        <v>('AR2880','Aerolineas Argentinas','Buenos Aires','bue-aep','San Salvador de Jujuy','ssj-juy','05-29-2019',NULL,1)</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q7">
+        <v>100</v>
+      </c>
+      <c r="R7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>('AR2880',2,'16:45:00','18:45:00',100)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2" t="str">
+        <f>CONCATENATE("(",A8,",",B8,",",C8,",",D8,",",E8,",",F8,",",G8,",",H8,",",I8,")")</f>
+        <v>('AR2881','Aerolineas Argentinas','San Salvador de Jujuy','ssj-juy','Buenos Aires','bue-aep','05-30-2019',NULL,1)</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q8">
+        <v>100</v>
+      </c>
+      <c r="R8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>('AR2881',2,'16:45:00','18:45:00',100)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9" s="2" t="str">
+        <f t="shared" ref="J9:J12" si="1">CONCATENATE("(",A9,",",B9,",",C9,",",D9,",",E9,",",F9,",",G9,",",H9,",",I9,")")</f>
+        <v>('AR2550','Aerolineas Argentinas','Buenos Aires','bue-aep','Ushuaia','tdf-uha','06-30-2019',NULL,2)</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N9">
+        <v>2</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q9">
+        <v>150</v>
+      </c>
+      <c r="R9" s="2" t="str">
+        <f t="shared" ref="R9:R12" si="2">CONCATENATE("(",M9,",",N9,",",O9,",",P9,",",Q9,")")</f>
+        <v>('AR2550',2,'18:45:00','20:45:00',150)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>('AR2551','Aerolineas Argentinas','Ushuaia','tdf-uha','Buenos Aires','bue-aep','06-30-2019',NULL,3)</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q10">
+        <v>150</v>
+      </c>
+      <c r="R10" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>('AR2551',2,'21:45:00','23:45:00',150)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>4</v>
+      </c>
+      <c r="J11" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>('AR2600','Aerolineas Argentinas','Buenos Aires','bue-aep','Mendoza','mdz-mdz','07-30-2019',NULL,4)</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q11">
+        <v>50</v>
+      </c>
+      <c r="R11" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>('AR2600',1,'17:45:00','18:45:00',50)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <v>5</v>
+      </c>
+      <c r="J12" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>('AR2601','Aerolineas Argentinas','San Salvador de Jujuy','ssj-juy','Buenos Aires','bue-aep','07-30-2019',NULL,5)</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q12">
+        <v>50</v>
+      </c>
+      <c r="R12" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>('AR2601',1,'19:45:00','20:45:00',50)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dos vuelos al mismo destino
</commit_message>
<xml_diff>
--- a/carga manual de vuelos.xlsx
+++ b/carga manual de vuelos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="74">
   <si>
     <t>'LAN'</t>
   </si>
@@ -219,6 +219,33 @@
   </si>
   <si>
     <t>'23:45:00'</t>
+  </si>
+  <si>
+    <t>'mdz-mdz</t>
+  </si>
+  <si>
+    <t>'FL143'</t>
+  </si>
+  <si>
+    <t>'7-30-2019'</t>
+  </si>
+  <si>
+    <t>'14:30:00'</t>
+  </si>
+  <si>
+    <t>'15:30:00'</t>
+  </si>
+  <si>
+    <t>'FL144'</t>
+  </si>
+  <si>
+    <t>'Flybondi'</t>
+  </si>
+  <si>
+    <t>'16:30:00'</t>
+  </si>
+  <si>
+    <t>'17:30:00'</t>
   </si>
 </sst>
 </file>
@@ -544,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" topLeftCell="D9" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -656,7 +683,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="2" t="str">
-        <f>CONCATENATE("(",A3,",",B3,",",C3,",",D3,",",E3,",",F3,",",G3,",",H3,",",I3,")")</f>
+        <f t="shared" ref="J3:J8" si="0">CONCATENATE("(",A3,",",B3,",",C3,",",D3,",",E3,",",F3,",",G3,",",H3,",",I3,")")</f>
         <v>('brrio01','LAN',Buenos Aires','bue-eze',Rio de Janeiro','bra-gig','06-23-2019',NULL,1)</v>
       </c>
       <c r="M3" s="1" t="s">
@@ -708,7 +735,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="2" t="str">
-        <f>CONCATENATE("(",A4,",",B4,",",C4,",",D4,",",E4,",",F4,",",G4,",",H4,",",I4,")")</f>
+        <f t="shared" si="0"/>
         <v>('brrio02','LAN',Rio de Janeiro','bra-gig',Buenos Aires',bue-eze','06-23-2019',NULL,1)</v>
       </c>
       <c r="M4" s="1" t="s">
@@ -760,7 +787,7 @@
         <v>1</v>
       </c>
       <c r="J5" s="2" t="str">
-        <f>CONCATENATE("(",A5,",",B5,",",C5,",",D5,",",E5,",",F5,",",G5,",",H5,",",I5,")")</f>
+        <f t="shared" si="0"/>
         <v>('DL101','Delta','Buenos Aires','bue-eze','Atlanta','atl-atl','08-26-2019',NULL,1)</v>
       </c>
       <c r="M5" s="1" t="s">
@@ -812,7 +839,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="2" t="str">
-        <f>CONCATENATE("(",A6,",",B6,",",C6,",",D6,",",E6,",",F6,",",G6,",",H6,",",I6,")")</f>
+        <f t="shared" si="0"/>
         <v>('DL102','Delta','Atlanta','atl-atl','Buenos Aires','bue-eze','08-30-2019',NULL,1)</v>
       </c>
       <c r="M6" s="1" t="s">
@@ -831,7 +858,7 @@
         <v>1300</v>
       </c>
       <c r="R6" s="2" t="str">
-        <f t="shared" ref="R6:R8" si="0">CONCATENATE("(",M6,",",N6,",",O6,",",P6,",",Q6,")")</f>
+        <f t="shared" ref="R6:R8" si="1">CONCATENATE("(",M6,",",N6,",",O6,",",P6,",",Q6,")")</f>
         <v>('DL102',10,'20:35:00','06:35:00',1300)</v>
       </c>
     </row>
@@ -864,7 +891,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="2" t="str">
-        <f>CONCATENATE("(",A7,",",B7,",",C7,",",D7,",",E7,",",F7,",",G7,",",H7,",",I7,")")</f>
+        <f t="shared" si="0"/>
         <v>('AR2880','Aerolineas Argentinas','Buenos Aires','bue-aep','San Salvador de Jujuy','ssj-juy','05-29-2019',NULL,1)</v>
       </c>
       <c r="M7" s="1" t="s">
@@ -883,7 +910,7 @@
         <v>100</v>
       </c>
       <c r="R7" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>('AR2880',2,'16:45:00','18:45:00',100)</v>
       </c>
     </row>
@@ -916,7 +943,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="2" t="str">
-        <f>CONCATENATE("(",A8,",",B8,",",C8,",",D8,",",E8,",",F8,",",G8,",",H8,",",I8,")")</f>
+        <f t="shared" si="0"/>
         <v>('AR2881','Aerolineas Argentinas','San Salvador de Jujuy','ssj-juy','Buenos Aires','bue-aep','05-30-2019',NULL,1)</v>
       </c>
       <c r="M8" s="1" t="s">
@@ -935,7 +962,7 @@
         <v>100</v>
       </c>
       <c r="R8" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>('AR2881',2,'16:45:00','18:45:00',100)</v>
       </c>
     </row>
@@ -965,11 +992,11 @@
         <v>4</v>
       </c>
       <c r="I9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9" s="2" t="str">
-        <f t="shared" ref="J9:J12" si="1">CONCATENATE("(",A9,",",B9,",",C9,",",D9,",",E9,",",F9,",",G9,",",H9,",",I9,")")</f>
-        <v>('AR2550','Aerolineas Argentinas','Buenos Aires','bue-aep','Ushuaia','tdf-uha','06-30-2019',NULL,2)</v>
+        <f t="shared" ref="J9:J14" si="2">CONCATENATE("(",A9,",",B9,",",C9,",",D9,",",E9,",",F9,",",G9,",",H9,",",I9,")")</f>
+        <v>('AR2550','Aerolineas Argentinas','Buenos Aires','bue-aep','Ushuaia','tdf-uha','06-30-2019',NULL,1)</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>50</v>
@@ -987,7 +1014,7 @@
         <v>150</v>
       </c>
       <c r="R9" s="2" t="str">
-        <f t="shared" ref="R9:R12" si="2">CONCATENATE("(",M9,",",N9,",",O9,",",P9,",",Q9,")")</f>
+        <f t="shared" ref="R9:R13" si="3">CONCATENATE("(",M9,",",N9,",",O9,",",P9,",",Q9,")")</f>
         <v>('AR2550',2,'18:45:00','20:45:00',150)</v>
       </c>
     </row>
@@ -1017,11 +1044,11 @@
         <v>4</v>
       </c>
       <c r="I10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J10" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>('AR2551','Aerolineas Argentinas','Ushuaia','tdf-uha','Buenos Aires','bue-aep','06-30-2019',NULL,3)</v>
+        <f t="shared" si="2"/>
+        <v>('AR2551','Aerolineas Argentinas','Ushuaia','tdf-uha','Buenos Aires','bue-aep','06-30-2019',NULL,1)</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>51</v>
@@ -1039,7 +1066,7 @@
         <v>150</v>
       </c>
       <c r="R10" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>('AR2551',2,'21:45:00','23:45:00',150)</v>
       </c>
     </row>
@@ -1069,11 +1096,11 @@
         <v>4</v>
       </c>
       <c r="I11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J11" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>('AR2600','Aerolineas Argentinas','Buenos Aires','bue-aep','Mendoza','mdz-mdz','07-30-2019',NULL,4)</v>
+        <f t="shared" si="2"/>
+        <v>('AR2600','Aerolineas Argentinas','Buenos Aires','bue-aep','Mendoza','mdz-mdz','07-30-2019',NULL,1)</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>52</v>
@@ -1091,7 +1118,7 @@
         <v>50</v>
       </c>
       <c r="R11" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>('AR2600',1,'17:45:00','18:45:00',50)</v>
       </c>
     </row>
@@ -1103,10 +1130,10 @@
         <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>31</v>
@@ -1121,11 +1148,11 @@
         <v>4</v>
       </c>
       <c r="I12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J12" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>('AR2601','Aerolineas Argentinas','San Salvador de Jujuy','ssj-juy','Buenos Aires','bue-aep','07-30-2019',NULL,5)</v>
+        <f t="shared" si="2"/>
+        <v>('AR2601','Aerolineas Argentinas','Mendoza','mdz-mdz,'Buenos Aires','bue-aep','07-30-2019',NULL,1)</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>53</v>
@@ -1143,8 +1170,112 @@
         <v>50</v>
       </c>
       <c r="R12" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>('AR2601',1,'19:45:00','20:45:00',50)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>('AR2601',1,'19:45:00','20:45:00',50)</v>
+        <v>('FL143','Flybondi','Buenos Aires','bue-aep','Mendoza','mdz-mdz','7-30-2019',NULL,1)</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q13">
+        <v>10</v>
+      </c>
+      <c r="R13" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>('FL143',1,'14:30:00','15:30:00',10)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>('FL144','Flybondi','Mendoza','mdz-mdz','Buenos Aires','bue-aep','7-30-2019',NULL,2)</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N14">
+        <v>2</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q14">
+        <v>12</v>
+      </c>
+      <c r="R14" s="2" t="str">
+        <f t="shared" ref="R14" si="4">CONCATENATE("(",M14,",",N14,",",O14,",",P14,",",Q14,")")</f>
+        <v>('FL144',2,'16:30:00','17:30:00',12)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>